<commit_message>
updated the KPI file
</commit_message>
<xml_diff>
--- a/目标考核/部门KPI－2013 Q3V001.xlsx
+++ b/目标考核/部门KPI－2013 Q3V001.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="16035" windowHeight="5970" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="16040" windowHeight="5980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="部门KPI" sheetId="10" r:id="rId1"/>
     <sheet name="Q3WIG" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>部门</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,10 +162,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>战斗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>目标</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -339,27 +340,33 @@
     <t>主管和员工每两周一次正式沟通；
 主管和团队每个月一起吃一顿饭；</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>员工敬业度</t>
+  </si>
+  <si>
+    <t>每个员工每周加2天班</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -373,7 +380,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -382,14 +389,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -398,7 +405,7 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -406,7 +413,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -421,7 +428,7 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -431,7 +438,7 @@
       <i/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -440,7 +447,7 @@
       <i/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -450,7 +457,7 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -481,6 +488,13 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
@@ -533,22 +547,22 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -558,7 +572,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -567,99 +581,99 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,18 +682,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,9 +704,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,23 +773,26 @@
     <xf numFmtId="9" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -807,34 +824,28 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="2"/>
     <cellStyle name="千位分隔 2" xfId="3"/>
   </cellStyles>
@@ -1132,83 +1143,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L229"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="34.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="48.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="34.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="48.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-    </row>
-    <row r="3" spans="1:12" s="18" customFormat="1" ht="36">
+      <c r="A2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" s="18" customFormat="1" ht="39">
       <c r="A3" s="14" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1255,7 @@
       </c>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:12" s="18" customFormat="1" ht="24">
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="39">
       <c r="A4" s="14" t="s">
         <v>17</v>
       </c>
@@ -1284,47 +1295,47 @@
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1"/>
     <row r="6" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-    </row>
-    <row r="229" spans="1:4" ht="12.75" thickBot="1">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+    </row>
+    <row r="229" spans="1:4" ht="15" thickBot="1">
       <c r="A229" s="8"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
@@ -1332,11 +1343,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
@@ -1349,349 +1355,362 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.75" style="22" customWidth="1"/>
-    <col min="3" max="3" width="43.875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="43.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="105.75" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="22"/>
+    <col min="1" max="2" width="13" style="40"/>
+    <col min="3" max="3" width="18" style="40" customWidth="1"/>
+    <col min="4" max="4" width="37" style="40" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" style="40" customWidth="1"/>
+    <col min="7" max="16384" width="13" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:8" ht="45">
+      <c r="A2" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" ht="33">
-      <c r="A2" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="D3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="24"/>
+      <c r="B4" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="24"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="24"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="23"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="27" t="s">
+      <c r="D6" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="24"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="24"/>
+      <c r="B8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="24"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="24"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="24"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" ht="30">
+      <c r="A14" s="24"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="24"/>
+      <c r="B15" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" ht="60">
+      <c r="A16" s="24"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="23"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="23"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="23"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8" ht="33">
-      <c r="A8" s="23"/>
-      <c r="B8" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="23"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="23"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="23"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="23"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="1:8" ht="49.5">
-      <c r="A16" s="23"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="23" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" ht="90">
+      <c r="A17" s="24"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D17" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="1:8" ht="66">
-      <c r="A17" s="23"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="23" t="s">
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:8" ht="45">
+      <c r="A18" s="24"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" ht="30">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="40" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>